<commit_message>
set components params content
</commit_message>
<xml_diff>
--- a/работа.xlsx
+++ b/работа.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="150">
   <si>
     <t>процесс</t>
   </si>
@@ -499,16 +499,19 @@
     <t>сброс данныз в бд + сброс индексы</t>
   </si>
   <si>
-    <t>components router params type = content</t>
-  </si>
-  <si>
     <t>делать валидацию что body совпадает с ожиданиемым интерфейсом</t>
   </si>
   <si>
-    <t>components router params type = var</t>
-  </si>
-  <si>
     <t>проверять каждый объект что он валиден и существует переменные могут не передаваться</t>
+  </si>
+  <si>
+    <t>баг body пустой объект</t>
+  </si>
+  <si>
+    <t>components  params type = content</t>
+  </si>
+  <si>
+    <t>components  params type = var</t>
   </si>
 </sst>
 </file>
@@ -1154,10 +1157,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1214,7 @@
       </c>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>10</v>
       </c>
@@ -1247,7 +1250,7 @@
       </c>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
@@ -1337,7 +1340,7 @@
       </c>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1471,7 @@
       <c r="F17" s="22"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>72</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>58</v>
       </c>
@@ -1779,7 +1782,7 @@
       </c>
       <c r="F34" s="20"/>
     </row>
-    <row r="35" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>100</v>
       </c>
@@ -1998,7 +2001,7 @@
       </c>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>59</v>
       </c>
@@ -2169,18 +2172,26 @@
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F63" s="35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F63" s="35" t="s">
-        <v>148</v>
+      <c r="B64" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
elemId max and set elemId new elements
</commit_message>
<xml_diff>
--- a/работа.xlsx
+++ b/работа.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Лист1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">общее!$C$1:$C$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">общее!$C$1:$C$64</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="150">
   <si>
     <t>процесс</t>
   </si>
@@ -475,9 +475,6 @@
     <t>webSocket chat</t>
   </si>
   <si>
-    <t>валидация web socket</t>
-  </si>
-  <si>
     <t>router style</t>
   </si>
   <si>
@@ -505,13 +502,16 @@
     <t>проверять каждый объект что он валиден и существует переменные могут не передаваться</t>
   </si>
   <si>
-    <t>баг body пустой объект</t>
-  </si>
-  <si>
     <t>components  params type = content</t>
   </si>
   <si>
     <t>components  params type = var</t>
+  </si>
+  <si>
+    <t>валидация web socket проверить на фронте!</t>
+  </si>
+  <si>
+    <t>полный функ компонентов</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +1962,7 @@
         <v>135</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
         <v>26</v>
       </c>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>59</v>
       </c>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>117</v>
       </c>
@@ -2031,7 +2031,7 @@
       <c r="E51" s="27"/>
       <c r="F51" s="28"/>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>62</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>65</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="F53" s="38"/>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>35</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>119</v>
       </c>
@@ -2099,9 +2099,9 @@
       <c r="E55" s="29"/>
       <c r="F55" s="30"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B56" s="36"/>
       <c r="C56" s="36" t="s">
@@ -2111,7 +2111,7 @@
       <c r="E56" s="36"/>
       <c r="F56" s="37"/>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>57</v>
       </c>
@@ -2122,12 +2122,12 @@
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="36" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
-        <v>140</v>
       </c>
       <c r="B58" s="36"/>
       <c r="C58" s="36" t="s">
@@ -2137,17 +2137,23 @@
       <c r="E58" s="36"/>
       <c r="F58" s="37"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="B60" s="36" t="s">
         <v>142</v>
-      </c>
-      <c r="B60" s="36" t="s">
-        <v>143</v>
       </c>
       <c r="C60" s="36" t="s">
         <v>4</v>
@@ -2156,12 +2162,12 @@
       <c r="E60" s="36"/>
       <c r="F60" s="37"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" s="36" t="s">
         <v>4</v>
@@ -2170,32 +2176,29 @@
       <c r="E61" s="36"/>
       <c r="F61" s="37"/>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F62" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F63" s="35" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F63" s="35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>147</v>
-      </c>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C57">
+  <autoFilter ref="C1:C64">
     <filterColumn colId="0">
       <filters blank="1">
         <filter val="возможные баги"/>

</xml_diff>

<commit_message>
support categories save and get
</commit_message>
<xml_diff>
--- a/работа.xlsx
+++ b/работа.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="общее" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="163">
   <si>
     <t>процесс</t>
   </si>
@@ -547,6 +547,9 @@
   </si>
   <si>
     <t>components params update ids</t>
+  </si>
+  <si>
+    <t>доработать поиск support по категории type support и создание в support категории type support</t>
   </si>
 </sst>
 </file>
@@ -1176,8 +1179,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,6 +1981,9 @@
       <c r="B47" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="C47" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="F47" s="29" t="s">
         <v>147</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>27</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D48" s="23" t="s">
         <v>7</v>
@@ -2008,7 +2014,7 @@
         <v>28</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D49" s="23" t="s">
         <v>7</v>
@@ -2108,7 +2114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>119</v>
       </c>
@@ -2116,11 +2122,13 @@
         <v>155</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
-      <c r="F55" s="27"/>
+      <c r="F55" s="27" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
@@ -2423,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bag support get categories IN
</commit_message>
<xml_diff>
--- a/работа.xlsx
+++ b/работа.xlsx
@@ -549,7 +549,7 @@
     <t>components params update ids</t>
   </si>
   <si>
-    <t>доработать поиск support по категории type support и создание в support категории type support</t>
+    <t>доработать поиск support по категории type</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
fix todo and support where sqlCategories
</commit_message>
<xml_diff>
--- a/работа.xlsx
+++ b/работа.xlsx
@@ -549,7 +549,7 @@
     <t>components params update ids</t>
   </si>
   <si>
-    <t>доработать поиск support по категории type</t>
+    <t>доработать поиск support по категории type и поле title</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
         <v>119</v>
       </c>

</xml_diff>